<commit_message>
Fixed property calculation bug, process removal bug, code cleanup
</commit_message>
<xml_diff>
--- a/TestCaseMatrix.xlsx
+++ b/TestCaseMatrix.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjorn/Documents/MATLAB/Git/MATLABToolKit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB8F3C-5981-C34A-B14B-8F0C8F562F39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F71F47-08F3-F64E-82B3-4F353A1394B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1860" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{66A0800E-5637-7549-822B-237FA3A774A7}"/>
+    <workbookView xWindow="10520" yWindow="500" windowWidth="16140" windowHeight="16320" xr2:uid="{66A0800E-5637-7549-822B-237FA3A774A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="20">
   <si>
     <t>P</t>
   </si>
@@ -88,6 +90,12 @@
   </si>
   <si>
     <t>high temp, low press</t>
+  </si>
+  <si>
+    <t>lower press than table range</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -136,16 +144,151 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.749961851863155"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -154,11 +297,36 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="8" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -179,6 +347,26 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="8" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -254,271 +442,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -832,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87532D3-4A08-094A-9DA5-38EEB2211AF9}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E19"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,7 +767,7 @@
     <col min="2" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -861,10 +784,13 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -872,19 +798,22 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>270</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+        <v>1.3017736E-3</v>
+      </c>
+      <c r="F2">
+        <v>2.9750999999999999</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -892,19 +821,22 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>170</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>280</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+        <v>1.3047934E-3</v>
+      </c>
+      <c r="F3">
+        <v>3.0356999999999998</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -912,79 +844,94 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>220</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+        <f>1.00033*10^-3</f>
+        <v>1.00033E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.151</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f>0.000000011143 * 10^5</f>
+        <v>1.1142999999999999E-3</v>
+      </c>
+      <c r="F5">
+        <v>2.0419</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <f>0.009351139325843*10^2</f>
+        <v>0.93511393258429998</v>
+      </c>
+      <c r="F6">
+        <v>7.1609999999999996</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>240</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>760</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.8823034299999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>6.8548</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -992,79 +939,84 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>650</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <f>0.00728775*10^2</f>
+        <v>0.72877499999999995</v>
+      </c>
+      <c r="F8">
+        <v>8.3955000000000002</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>8.1300000000000001E-3</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1.000168*1.1*10^-3</f>
+        <v>1.1001848000000002E-3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>15.54</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.05</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>7.3840000000000003E-2</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1080,11 +1032,11 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1100,16 +1052,16 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1120,11 +1072,11 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1140,11 +1092,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1160,16 +1112,16 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1180,11 +1132,11 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1200,11 +1152,11 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1220,60 +1172,609 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A6 A8 A20:A1048576">
-    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="R134a">
+  <conditionalFormatting sqref="A2:A4 A6 A21:A1048576 A8:A11">
+    <cfRule type="containsText" dxfId="33" priority="23" operator="containsText" text="R134a">
       <formula>NOT(ISERROR(SEARCH("R134a",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="19" operator="containsText" text="Water">
+    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="Water">
       <formula>NOT(ISERROR(SEARCH("Water",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="containsText" dxfId="31" priority="21" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="22" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="R134a">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="R134a">
       <formula>NOT(ISERROR(SEARCH("R134a",A7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="17" operator="containsText" text="Water">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="Water">
       <formula>NOT(ISERROR(SEARCH("Water",A7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="R134a">
-      <formula>NOT(ISERROR(SEARCH("R134a",A9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Water">
-      <formula>NOT(ISERROR(SEARCH("Water",A9)))</formula>
+  <conditionalFormatting sqref="A12:A20">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="16" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="R134a">
-      <formula>NOT(ISERROR(SEARCH("R134a",A10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="13" operator="containsText" text="Water">
-      <formula>NOT(ISERROR(SEARCH("Water",A10)))</formula>
+  <conditionalFormatting sqref="B2:G4 B24:G1048576 D23:G23 B23 B6:G22">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Mix">
+      <formula>NOT(ISERROR(SEARCH("Mix",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="Vapor">
+      <formula>NOT(ISERROR(SEARCH("Vapor",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="Liquid">
+      <formula>NOT(ISERROR(SEARCH("Liquid",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A19">
-    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="R134a">
+  <conditionalFormatting sqref="A5">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:G5">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Mix">
+      <formula>NOT(ISERROR(SEARCH("Mix",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Vapor">
+      <formula>NOT(ISERROR(SEARCH("Vapor",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Liquid">
+      <formula>NOT(ISERROR(SEARCH("Liquid",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC4B432-7CA8-CC46-836D-C623B3BFED88}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="3" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>270</v>
+      </c>
+      <c r="E2">
+        <v>1.3017736E-3</v>
+      </c>
+      <c r="F2">
+        <v>2.9746711372000001</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>170</v>
+      </c>
+      <c r="D3">
+        <v>280</v>
+      </c>
+      <c r="E3">
+        <v>1.3047934E-3</v>
+      </c>
+      <c r="F3">
+        <v>3.0346460653</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>220</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f>1.00033*10^-3</f>
+        <v>1.00033E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.14859390359999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>170</v>
+      </c>
+      <c r="E5">
+        <f>0.000000011143 * 10^5</f>
+        <v>1.1142999999999999E-3</v>
+      </c>
+      <c r="F5">
+        <v>2.0416565213000002</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>125</v>
+      </c>
+      <c r="E6">
+        <f>0.009351139325843*10^2</f>
+        <v>0.93511393258429998</v>
+      </c>
+      <c r="F6">
+        <v>7.1529906861999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>240</v>
+      </c>
+      <c r="D7">
+        <v>760</v>
+      </c>
+      <c r="E7">
+        <v>1.8823034299999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>6.8546549514999997</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>650</v>
+      </c>
+      <c r="E8">
+        <f>0.00728775*10^2</f>
+        <v>0.72877499999999995</v>
+      </c>
+      <c r="F8">
+        <v>8.4783701059999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>8.1300000000000001E-3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f>1.000168*1.1*10^-3</f>
+        <v>1.1001848000000002E-3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>15.54</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>7.3840000000000003E-2</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B5:G5">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Mix">
+      <formula>NOT(ISERROR(SEARCH("Mix",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Vapor">
+      <formula>NOT(ISERROR(SEARCH("Vapor",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Liquid">
+      <formula>NOT(ISERROR(SEARCH("Liquid",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A4 A6 A9:A10">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="R134a">
       <formula>NOT(ISERROR(SEARCH("R134a",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="Water">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Water">
       <formula>NOT(ISERROR(SEARCH("Water",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F1048576">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Liquid">
+  <conditionalFormatting sqref="A7">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A11">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:A20">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G4 B6:G20">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Mix">
+      <formula>NOT(ISERROR(SEARCH("Mix",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Vapor">
+      <formula>NOT(ISERROR(SEARCH("Vapor",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Liquid">
       <formula>NOT(ISERROR(SEARCH("Liquid",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="Vapor">
-      <formula>NOT(ISERROR(SEARCH("Vapor",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Mix">
-      <formula>NOT(ISERROR(SEARCH("Mix",B2)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="R134a">
+      <formula>NOT(ISERROR(SEARCH("R134a",A5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Water">
+      <formula>NOT(ISERROR(SEARCH("Water",A5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>